<commit_message>
Module 17 Challenge complete
</commit_message>
<xml_diff>
--- a/Images/other.xlsx
+++ b/Images/other.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luispsalazar/Desktop/Credit_Risk_Analysis/Images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF9DB7A-E6C4-314E-98F8-5EB3FE4F0700}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA002C4-4BAC-4E46-8589-5EF0FC66EB70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51220" yWindow="-5260" windowWidth="25600" windowHeight="28300" activeTab="1" xr2:uid="{B1119282-89D9-874B-AA51-8E7AF1AB04E9}"/>
+    <workbookView xWindow="20600" yWindow="500" windowWidth="20360" windowHeight="22540" activeTab="4" xr2:uid="{B1119282-89D9-874B-AA51-8E7AF1AB04E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1 (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>SMOTE Oversampling</t>
   </si>
@@ -40,12 +42,66 @@
   <si>
     <t>Random Oversampler</t>
   </si>
+  <si>
+    <t>RandomOverSampler</t>
+  </si>
+  <si>
+    <t>SMOTE</t>
+  </si>
+  <si>
+    <t>ClusterCentroids</t>
+  </si>
+  <si>
+    <t>BalancedRandomForestClassifier</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>F1 score</t>
+  </si>
+  <si>
+    <t>Low Risk</t>
+  </si>
+  <si>
+    <t>Deliverable</t>
+  </si>
+  <si>
+    <t>SMOTEENN</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>EasyEnsembleClassifier</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>sensiti</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>High Risk</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -60,16 +116,69 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -77,18 +186,375 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -644,6 +1110,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>274370</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC6B0A2E-602D-E945-A0FA-4C30CBD8FC2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="787400" y="368300"/>
+          <a:ext cx="4439970" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>392252</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7ECF033-C2C0-864D-A31E-32E876E5E7A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5422900" y="406400"/>
+          <a:ext cx="5700852" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -947,24 +1506,24 @@
       <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="5" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:2" ht="29">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:2" ht="29">
       <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:2" ht="29">
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" ht="29">
       <c r="B35" s="1" t="s">
         <v>2</v>
       </c>
@@ -979,28 +1538,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8F424B-BB5F-5548-8FE8-C9809095FD0F}">
   <dimension ref="B5:B55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="5" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:2" ht="29">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2" ht="29">
       <c r="B22" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" ht="29">
       <c r="B38" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:2" ht="29">
       <c r="B55" s="1" t="s">
         <v>2</v>
       </c>
@@ -1019,24 +1578,24 @@
       <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="5" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:2" ht="29">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" ht="29">
       <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" ht="29">
       <c r="B36" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:2" ht="29">
       <c r="B50" s="1" t="s">
         <v>2</v>
       </c>
@@ -1045,4 +1604,427 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F732F58B-AA2B-7944-85A7-2240D2D40553}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8677BE23-EDB8-9F4F-930C-977BD3961D6D}">
+  <dimension ref="B5:J24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <cols>
+    <col min="1" max="1" width="7" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="12.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:10" ht="21" thickBot="1"/>
+    <row r="6" spans="2:10" ht="21" thickTop="1">
+      <c r="B6" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="31"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0.65339000000000003</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.63</v>
+      </c>
+      <c r="G8" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="H8" s="18">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.67</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.65122000000000002</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.64</v>
+      </c>
+      <c r="G9" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="H9" s="18">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.66</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0.52939000000000003</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.61</v>
+      </c>
+      <c r="G10" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="H10" s="18">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" s="10" customFormat="1" ht="9">
+      <c r="B11" s="33"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="7">
+        <v>2</v>
+      </c>
+      <c r="D12" s="15">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.69</v>
+      </c>
+      <c r="G12" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="H12" s="18">
+        <v>1</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" s="10" customFormat="1" ht="9">
+      <c r="B13" s="33"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7">
+        <v>3</v>
+      </c>
+      <c r="D14" s="15">
+        <v>0.78769999999999996</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.67</v>
+      </c>
+      <c r="G14" s="25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H14" s="18">
+        <v>1</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.91</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="21" thickBot="1">
+      <c r="B15" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="7">
+        <v>3</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0.9254</v>
+      </c>
+      <c r="E15" s="28">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F15" s="29">
+        <v>0.91</v>
+      </c>
+      <c r="G15" s="30">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H15" s="18">
+        <v>1</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.94</v>
+      </c>
+      <c r="J15" s="6">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="21" thickTop="1"/>
+    <row r="20" spans="2:10">
+      <c r="C20" s="4">
+        <v>79</v>
+      </c>
+      <c r="D20" s="4">
+        <v>8</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="11">
+        <f>C20/(C20+D20)</f>
+        <v>0.90804597701149425</v>
+      </c>
+      <c r="I20" s="12"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="C21" s="4">
+        <v>979</v>
+      </c>
+      <c r="D21" s="4">
+        <v>16139</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="11">
+        <f>C20/(C20+C21)</f>
+        <v>7.4669187145557661E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="F24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="11">
+        <f>2*C23*G20/(C23+G20)</f>
+        <v>0.13799126637554585</v>
+      </c>
+      <c r="I24" s="12"/>
+      <c r="J24" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="H6:J6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D8:D15">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{47704ED9-A170-EB46-AAF0-6A443F889701}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:G15">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B21FD536-9B84-6644-AE70-15B53B340B90}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8:J15">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B6943B32-F716-9E43-920F-66993A6ABA1C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{47704ED9-A170-EB46-AAF0-6A443F889701}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D8:D15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B21FD536-9B84-6644-AE70-15B53B340B90}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E8:G15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B6943B32-F716-9E43-920F-66993A6ABA1C}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I8:J15</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>